<commit_message>
Vistas Tools by Job
</commit_message>
<xml_diff>
--- a/Documentacion/Warehouse Inventory.xlsx
+++ b/Documentacion/Warehouse Inventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="887"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="887" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Rescue Kits" sheetId="2" r:id="rId1"/>
@@ -1026,9 +1026,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3857,7 +3857,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3988,9 +3988,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,7 +4150,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>